<commit_message>
Fix bad names of features. Add indexes to FindFeatures.xlsx
</commit_message>
<xml_diff>
--- a/Docs/FindFeatures.xlsx
+++ b/Docs/FindFeatures.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dzmitry_Rybalko\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositroies\TechAnalyzer\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -910,9 +910,6 @@
     <t>WeakMap</t>
   </si>
   <si>
-    <t xml:space="preserve">Uievents </t>
-  </si>
-  <si>
     <t>Multimedia</t>
   </si>
   <si>
@@ -1616,6 +1613,9 @@
   </si>
   <si>
     <t>Id</t>
+  </si>
+  <si>
+    <t>Uievents - Keyboard Query APIs</t>
   </si>
 </sst>
 </file>
@@ -1988,8 +1988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F207"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="A210" sqref="A210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2002,7 +2002,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
@@ -2186,6 +2186,9 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>204</v>
+      </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -2299,6 +2302,9 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>173</v>
+      </c>
       <c r="B19" t="s">
         <v>10</v>
       </c>
@@ -2630,6 +2636,9 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>152</v>
+      </c>
       <c r="B39" t="s">
         <v>10</v>
       </c>
@@ -2734,6 +2743,9 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>179</v>
+      </c>
       <c r="B46" t="s">
         <v>121</v>
       </c>
@@ -2864,6 +2876,9 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>185</v>
+      </c>
       <c r="B54" t="s">
         <v>136</v>
       </c>
@@ -2920,6 +2935,9 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>156</v>
+      </c>
       <c r="B58" t="s">
         <v>161</v>
       </c>
@@ -2982,6 +3000,9 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>189</v>
+      </c>
       <c r="B62" t="s">
         <v>170</v>
       </c>
@@ -2989,10 +3010,13 @@
         <v>171</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>184</v>
+      </c>
       <c r="B63" t="s">
         <v>170</v>
       </c>
@@ -3004,6 +3028,9 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>191</v>
+      </c>
       <c r="B64" t="s">
         <v>170</v>
       </c>
@@ -3043,6 +3070,9 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>192</v>
+      </c>
       <c r="B67" t="s">
         <v>170</v>
       </c>
@@ -3057,6 +3087,9 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>159</v>
+      </c>
       <c r="B68" t="s">
         <v>170</v>
       </c>
@@ -3076,6 +3109,9 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>163</v>
+      </c>
       <c r="B70" t="s">
         <v>170</v>
       </c>
@@ -3090,6 +3126,9 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>162</v>
+      </c>
       <c r="B71" t="s">
         <v>170</v>
       </c>
@@ -3115,6 +3154,9 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>161</v>
+      </c>
       <c r="B73" t="s">
         <v>170</v>
       </c>
@@ -3188,6 +3230,9 @@
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>196</v>
+      </c>
       <c r="B78" t="s">
         <v>170</v>
       </c>
@@ -3213,6 +3258,9 @@
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>151</v>
+      </c>
       <c r="B80" t="s">
         <v>207</v>
       </c>
@@ -3294,6 +3342,9 @@
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>165</v>
+      </c>
       <c r="B86" t="s">
         <v>207</v>
       </c>
@@ -3325,6 +3376,9 @@
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>158</v>
+      </c>
       <c r="B88" t="s">
         <v>207</v>
       </c>
@@ -3333,6 +3387,9 @@
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>174</v>
+      </c>
       <c r="B89" t="s">
         <v>207</v>
       </c>
@@ -3344,6 +3401,9 @@
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>183</v>
+      </c>
       <c r="B90" t="s">
         <v>207</v>
       </c>
@@ -3372,6 +3432,9 @@
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>166</v>
+      </c>
       <c r="B92" t="s">
         <v>207</v>
       </c>
@@ -3380,6 +3443,9 @@
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>153</v>
+      </c>
       <c r="B93" t="s">
         <v>207</v>
       </c>
@@ -3504,6 +3570,9 @@
       </c>
     </row>
     <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>157</v>
+      </c>
       <c r="B101" t="s">
         <v>207</v>
       </c>
@@ -3514,7 +3583,7 @@
         <v>258</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -3597,6 +3666,9 @@
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>168</v>
+      </c>
       <c r="B107" t="s">
         <v>207</v>
       </c>
@@ -3653,6 +3725,9 @@
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>155</v>
+      </c>
       <c r="B111" t="s">
         <v>207</v>
       </c>
@@ -3661,6 +3736,9 @@
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>182</v>
+      </c>
       <c r="B112" t="s">
         <v>207</v>
       </c>
@@ -3675,25 +3753,31 @@
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>175</v>
+      </c>
       <c r="B113" t="s">
+        <v>291</v>
+      </c>
+      <c r="C113" t="s">
+        <v>523</v>
+      </c>
+      <c r="E113" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="C113" t="s">
-        <v>291</v>
-      </c>
-      <c r="E113" s="4" t="s">
-        <v>293</v>
-      </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>188</v>
+      </c>
       <c r="B114" t="s">
         <v>279</v>
       </c>
       <c r="C114" t="s">
+        <v>293</v>
+      </c>
+      <c r="D114" s="4" t="s">
         <v>294</v>
-      </c>
-      <c r="D114" s="4" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -3704,7 +3788,7 @@
         <v>279</v>
       </c>
       <c r="C115" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3715,13 +3799,13 @@
         <v>279</v>
       </c>
       <c r="C116" t="s">
+        <v>296</v>
+      </c>
+      <c r="D116" t="s">
+        <v>298</v>
+      </c>
+      <c r="E116" s="3" t="s">
         <v>297</v>
-      </c>
-      <c r="D116" t="s">
-        <v>299</v>
-      </c>
-      <c r="E116" s="3" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -3732,10 +3816,10 @@
         <v>279</v>
       </c>
       <c r="C117" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E117" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -3763,13 +3847,13 @@
         <v>279</v>
       </c>
       <c r="C119" t="s">
+        <v>300</v>
+      </c>
+      <c r="D119" t="s">
         <v>301</v>
       </c>
-      <c r="D119" t="s">
+      <c r="E119" t="s">
         <v>302</v>
-      </c>
-      <c r="E119" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -3780,10 +3864,10 @@
         <v>279</v>
       </c>
       <c r="C120" t="s">
+        <v>303</v>
+      </c>
+      <c r="E120" s="4" t="s">
         <v>304</v>
-      </c>
-      <c r="E120" s="4" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -3791,16 +3875,16 @@
         <v>125</v>
       </c>
       <c r="B121" t="s">
+        <v>306</v>
+      </c>
+      <c r="C121" t="s">
+        <v>305</v>
+      </c>
+      <c r="D121" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="C121" t="s">
-        <v>306</v>
-      </c>
-      <c r="D121" s="4" t="s">
+      <c r="E121" t="s">
         <v>308</v>
-      </c>
-      <c r="E121" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -3811,13 +3895,13 @@
         <v>279</v>
       </c>
       <c r="C122" t="s">
+        <v>309</v>
+      </c>
+      <c r="D122" t="s">
         <v>310</v>
       </c>
-      <c r="D122" t="s">
+      <c r="E122" t="s">
         <v>311</v>
-      </c>
-      <c r="E122" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -3828,10 +3912,10 @@
         <v>279</v>
       </c>
       <c r="C123" t="s">
+        <v>312</v>
+      </c>
+      <c r="E123" t="s">
         <v>313</v>
-      </c>
-      <c r="E123" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -3842,13 +3926,13 @@
         <v>279</v>
       </c>
       <c r="C124" t="s">
+        <v>314</v>
+      </c>
+      <c r="D124" t="s">
         <v>315</v>
       </c>
-      <c r="D124" t="s">
+      <c r="E124" t="s">
         <v>316</v>
-      </c>
-      <c r="E124" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -3856,16 +3940,16 @@
         <v>109</v>
       </c>
       <c r="B125" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C125" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D125" t="s">
+        <v>319</v>
+      </c>
+      <c r="E125" t="s">
         <v>320</v>
-      </c>
-      <c r="E125" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3873,16 +3957,16 @@
         <v>70</v>
       </c>
       <c r="B126" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C126" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D126" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="E126" s="3" t="s">
         <v>322</v>
-      </c>
-      <c r="E126" s="3" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -3890,16 +3974,16 @@
         <v>3</v>
       </c>
       <c r="B127" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C127" t="s">
+        <v>323</v>
+      </c>
+      <c r="D127" t="s">
         <v>324</v>
       </c>
-      <c r="D127" t="s">
+      <c r="E127" t="s">
         <v>325</v>
-      </c>
-      <c r="E127" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -3907,16 +3991,16 @@
         <v>4</v>
       </c>
       <c r="B128" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C128" t="s">
+        <v>326</v>
+      </c>
+      <c r="D128" t="s">
         <v>327</v>
       </c>
-      <c r="D128" t="s">
+      <c r="E128" t="s">
         <v>328</v>
-      </c>
-      <c r="E128" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3924,13 +4008,13 @@
         <v>123</v>
       </c>
       <c r="B129" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C129" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D129" s="4" t="s">
         <v>330</v>
-      </c>
-      <c r="D129" s="4" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -3938,41 +4022,47 @@
         <v>86</v>
       </c>
       <c r="B130" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C130" t="s">
+        <v>331</v>
+      </c>
+      <c r="D130" t="s">
         <v>332</v>
       </c>
-      <c r="D130" t="s">
+      <c r="E130" t="s">
         <v>333</v>
       </c>
-      <c r="E130" t="s">
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>186</v>
+      </c>
+      <c r="B131" t="s">
+        <v>291</v>
+      </c>
+      <c r="C131" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B131" t="s">
-        <v>292</v>
-      </c>
-      <c r="C131" t="s">
+      <c r="D131" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="D131" s="4" t="s">
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>172</v>
+      </c>
+      <c r="B132" t="s">
+        <v>291</v>
+      </c>
+      <c r="C132" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B132" t="s">
-        <v>292</v>
-      </c>
-      <c r="C132" t="s">
+      <c r="D132" t="s">
         <v>337</v>
       </c>
-      <c r="D132" t="s">
+      <c r="E132" t="s">
         <v>338</v>
-      </c>
-      <c r="E132" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -3980,16 +4070,16 @@
         <v>112</v>
       </c>
       <c r="B133" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C133" t="s">
+        <v>339</v>
+      </c>
+      <c r="D133" t="s">
         <v>340</v>
       </c>
-      <c r="D133" t="s">
+      <c r="E133" t="s">
         <v>341</v>
-      </c>
-      <c r="E133" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -3997,24 +4087,27 @@
         <v>7</v>
       </c>
       <c r="B134" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C134" t="s">
+        <v>342</v>
+      </c>
+      <c r="E134" t="s">
         <v>343</v>
       </c>
-      <c r="E134" t="s">
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>180</v>
+      </c>
+      <c r="B135" t="s">
+        <v>291</v>
+      </c>
+      <c r="C135" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B135" t="s">
-        <v>292</v>
-      </c>
-      <c r="C135" t="s">
+      <c r="E135" t="s">
         <v>345</v>
-      </c>
-      <c r="E135" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -4022,27 +4115,30 @@
         <v>106</v>
       </c>
       <c r="B136" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C136" t="s">
+        <v>346</v>
+      </c>
+      <c r="E136" t="s">
         <v>347</v>
       </c>
-      <c r="E136" t="s">
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>195</v>
+      </c>
+      <c r="B137" t="s">
+        <v>291</v>
+      </c>
+      <c r="C137" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B137" t="s">
-        <v>292</v>
-      </c>
-      <c r="C137" t="s">
+      <c r="D137" t="s">
         <v>349</v>
       </c>
-      <c r="D137" t="s">
+      <c r="E137" t="s">
         <v>350</v>
-      </c>
-      <c r="E137" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -4050,24 +4146,27 @@
         <v>77</v>
       </c>
       <c r="B138" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C138" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>202</v>
+      </c>
+      <c r="B139" t="s">
+        <v>291</v>
+      </c>
+      <c r="C139" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B139" t="s">
-        <v>292</v>
-      </c>
-      <c r="C139" t="s">
+      <c r="D139" t="s">
+        <v>354</v>
+      </c>
+      <c r="E139" t="s">
         <v>353</v>
-      </c>
-      <c r="D139" t="s">
-        <v>355</v>
-      </c>
-      <c r="E139" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -4075,66 +4174,78 @@
         <v>61</v>
       </c>
       <c r="B140" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C140" t="s">
+        <v>355</v>
+      </c>
+      <c r="D140" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="D140" s="4" t="s">
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>193</v>
+      </c>
+      <c r="B141" t="s">
+        <v>291</v>
+      </c>
+      <c r="C141" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B141" t="s">
-        <v>292</v>
-      </c>
-      <c r="C141" t="s">
+      <c r="D141" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="D141" s="4" t="s">
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>181</v>
+      </c>
+      <c r="B142" t="s">
+        <v>291</v>
+      </c>
+      <c r="C142" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B142" t="s">
-        <v>292</v>
-      </c>
-      <c r="C142" t="s">
+      <c r="D142" t="s">
         <v>360</v>
       </c>
-      <c r="D142" t="s">
+      <c r="E142" t="s">
         <v>361</v>
       </c>
-      <c r="E142" t="s">
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>200</v>
+      </c>
+      <c r="B143" t="s">
+        <v>291</v>
+      </c>
+      <c r="C143" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B143" t="s">
-        <v>292</v>
-      </c>
-      <c r="C143" t="s">
+      <c r="D143" t="s">
         <v>363</v>
       </c>
-      <c r="D143" t="s">
+      <c r="E143" t="s">
         <v>364</v>
       </c>
-      <c r="E143" t="s">
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>201</v>
+      </c>
+      <c r="B144" t="s">
+        <v>291</v>
+      </c>
+      <c r="C144" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B144" t="s">
-        <v>292</v>
-      </c>
-      <c r="C144" t="s">
+      <c r="D144" t="s">
         <v>366</v>
       </c>
-      <c r="D144" t="s">
+      <c r="E144" t="s">
         <v>367</v>
-      </c>
-      <c r="E144" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -4142,16 +4253,16 @@
         <v>105</v>
       </c>
       <c r="B145" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C145" t="s">
+        <v>368</v>
+      </c>
+      <c r="D145" t="s">
         <v>369</v>
       </c>
-      <c r="D145" t="s">
-        <v>370</v>
-      </c>
       <c r="E145" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -4159,13 +4270,13 @@
         <v>83</v>
       </c>
       <c r="B146" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C146" t="s">
+        <v>370</v>
+      </c>
+      <c r="D146" s="4" t="s">
         <v>371</v>
-      </c>
-      <c r="D146" s="4" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -4173,16 +4284,16 @@
         <v>101</v>
       </c>
       <c r="B147" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C147" t="s">
+        <v>372</v>
+      </c>
+      <c r="D147" t="s">
         <v>373</v>
       </c>
-      <c r="D147" t="s">
+      <c r="E147" t="s">
         <v>374</v>
-      </c>
-      <c r="E147" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -4190,13 +4301,13 @@
         <v>102</v>
       </c>
       <c r="B148" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C148" t="s">
+        <v>375</v>
+      </c>
+      <c r="D148" s="4" t="s">
         <v>376</v>
-      </c>
-      <c r="D148" s="4" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -4204,41 +4315,47 @@
         <v>135</v>
       </c>
       <c r="B149" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C149" t="s">
+        <v>377</v>
+      </c>
+      <c r="D149" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="D149" s="4" t="s">
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>194</v>
+      </c>
+      <c r="B150" t="s">
+        <v>291</v>
+      </c>
+      <c r="C150" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B150" t="s">
-        <v>292</v>
-      </c>
-      <c r="C150" t="s">
+      <c r="D150" t="s">
+        <v>381</v>
+      </c>
+      <c r="E150" t="s">
         <v>380</v>
       </c>
-      <c r="D150" t="s">
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>164</v>
+      </c>
+      <c r="B151" t="s">
+        <v>291</v>
+      </c>
+      <c r="C151" t="s">
         <v>382</v>
       </c>
-      <c r="E150" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B151" t="s">
-        <v>292</v>
-      </c>
-      <c r="C151" t="s">
+      <c r="D151" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="D151" s="4" t="s">
+      <c r="E151" t="s">
         <v>384</v>
-      </c>
-      <c r="E151" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -4246,29 +4363,35 @@
         <v>81</v>
       </c>
       <c r="B152" t="s">
+        <v>386</v>
+      </c>
+      <c r="C152" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>154</v>
+      </c>
+      <c r="B153" t="s">
+        <v>386</v>
+      </c>
+      <c r="C153" t="s">
         <v>387</v>
       </c>
-      <c r="C152" t="s">
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>176</v>
+      </c>
+      <c r="B154" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B153" t="s">
-        <v>387</v>
-      </c>
-      <c r="C153" t="s">
+      <c r="C154" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B154" t="s">
-        <v>387</v>
-      </c>
-      <c r="C154" t="s">
+      <c r="D154" s="4" t="s">
         <v>389</v>
-      </c>
-      <c r="D154" s="4" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -4276,13 +4399,13 @@
         <v>133</v>
       </c>
       <c r="B155" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C155" t="s">
+        <v>390</v>
+      </c>
+      <c r="D155" s="4" t="s">
         <v>391</v>
-      </c>
-      <c r="D155" s="4" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -4290,30 +4413,33 @@
         <v>2</v>
       </c>
       <c r="B156" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C156" t="s">
+        <v>392</v>
+      </c>
+      <c r="D156" t="s">
         <v>393</v>
       </c>
-      <c r="D156" t="s">
+      <c r="E156" t="s">
         <v>394</v>
       </c>
-      <c r="E156" t="s">
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>205</v>
+      </c>
+      <c r="B157" t="s">
+        <v>386</v>
+      </c>
+      <c r="C157" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B157" t="s">
-        <v>387</v>
-      </c>
-      <c r="C157" t="s">
+      <c r="D157" t="s">
         <v>396</v>
       </c>
-      <c r="D157" t="s">
+      <c r="E157" t="s">
         <v>397</v>
-      </c>
-      <c r="E157" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -4321,13 +4447,13 @@
         <v>82</v>
       </c>
       <c r="B158" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C158" t="s">
+        <v>398</v>
+      </c>
+      <c r="D158" s="4" t="s">
         <v>399</v>
-      </c>
-      <c r="D158" s="4" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -4335,35 +4461,41 @@
         <v>65</v>
       </c>
       <c r="B159" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C159" t="s">
+        <v>400</v>
+      </c>
+      <c r="D159" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="D159" s="4" t="s">
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>170</v>
+      </c>
+      <c r="B160" t="s">
+        <v>386</v>
+      </c>
+      <c r="C160" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B160" t="s">
-        <v>387</v>
-      </c>
-      <c r="C160" t="s">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>199</v>
+      </c>
+      <c r="B161" t="s">
+        <v>386</v>
+      </c>
+      <c r="C161" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B161" t="s">
-        <v>387</v>
-      </c>
-      <c r="C161" t="s">
+      <c r="D161" t="s">
         <v>404</v>
       </c>
-      <c r="D161" t="s">
-        <v>405</v>
-      </c>
       <c r="E161" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="162" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -4371,30 +4503,33 @@
         <v>90</v>
       </c>
       <c r="B162" t="s">
+        <v>406</v>
+      </c>
+      <c r="C162" t="s">
+        <v>405</v>
+      </c>
+      <c r="D162" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="C162" t="s">
+      <c r="E162" s="3" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>203</v>
+      </c>
+      <c r="B163" t="s">
         <v>406</v>
       </c>
-      <c r="D162" s="3" t="s">
-        <v>408</v>
-      </c>
-      <c r="E162" s="3" t="s">
+      <c r="C163" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B163" t="s">
-        <v>407</v>
-      </c>
-      <c r="C163" t="s">
+      <c r="D163" t="s">
         <v>410</v>
       </c>
-      <c r="D163" t="s">
+      <c r="E163" t="s">
         <v>411</v>
-      </c>
-      <c r="E163" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -4402,16 +4537,16 @@
         <v>147</v>
       </c>
       <c r="B164" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C164" t="s">
+        <v>412</v>
+      </c>
+      <c r="D164" t="s">
         <v>413</v>
       </c>
-      <c r="D164" t="s">
+      <c r="E164" t="s">
         <v>414</v>
-      </c>
-      <c r="E164" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -4419,16 +4554,16 @@
         <v>140</v>
       </c>
       <c r="B165" t="s">
+        <v>416</v>
+      </c>
+      <c r="C165" t="s">
+        <v>415</v>
+      </c>
+      <c r="D165" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="C165" t="s">
-        <v>416</v>
-      </c>
-      <c r="D165" s="4" t="s">
+      <c r="E165" t="s">
         <v>418</v>
-      </c>
-      <c r="E165" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -4436,13 +4571,13 @@
         <v>116</v>
       </c>
       <c r="B166" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C166" t="s">
+        <v>419</v>
+      </c>
+      <c r="D166" s="4" t="s">
         <v>420</v>
-      </c>
-      <c r="D166" s="4" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -4450,13 +4585,13 @@
         <v>139</v>
       </c>
       <c r="B167" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C167" t="s">
+        <v>421</v>
+      </c>
+      <c r="D167" s="4" t="s">
         <v>422</v>
-      </c>
-      <c r="D167" s="4" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -4464,13 +4599,13 @@
         <v>78</v>
       </c>
       <c r="B168" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C168" t="s">
+        <v>423</v>
+      </c>
+      <c r="D168" s="4" t="s">
         <v>424</v>
-      </c>
-      <c r="D168" s="4" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -4478,27 +4613,30 @@
         <v>9</v>
       </c>
       <c r="B169" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C169" t="s">
+        <v>425</v>
+      </c>
+      <c r="D169" t="s">
         <v>426</v>
       </c>
-      <c r="D169" t="s">
+      <c r="E169" t="s">
         <v>427</v>
       </c>
-      <c r="E169" t="s">
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>178</v>
+      </c>
+      <c r="B170" t="s">
+        <v>416</v>
+      </c>
+      <c r="C170" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B170" t="s">
-        <v>417</v>
-      </c>
-      <c r="C170" t="s">
+      <c r="D170" s="4" t="s">
         <v>429</v>
-      </c>
-      <c r="D170" s="4" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -4506,16 +4644,16 @@
         <v>128</v>
       </c>
       <c r="B171" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C171" t="s">
+        <v>430</v>
+      </c>
+      <c r="D171" t="s">
         <v>431</v>
       </c>
-      <c r="D171" t="s">
+      <c r="E171" t="s">
         <v>432</v>
-      </c>
-      <c r="E171" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -4523,13 +4661,13 @@
         <v>129</v>
       </c>
       <c r="B172" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C172" t="s">
+        <v>433</v>
+      </c>
+      <c r="D172" s="4" t="s">
         <v>434</v>
-      </c>
-      <c r="D172" s="4" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -4537,13 +4675,13 @@
         <v>115</v>
       </c>
       <c r="B173" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C173" t="s">
+        <v>435</v>
+      </c>
+      <c r="D173" s="4" t="s">
         <v>436</v>
-      </c>
-      <c r="D173" s="4" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -4554,7 +4692,7 @@
         <v>10</v>
       </c>
       <c r="C174" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
@@ -4562,27 +4700,30 @@
         <v>107</v>
       </c>
       <c r="B175" t="s">
+        <v>439</v>
+      </c>
+      <c r="C175" t="s">
+        <v>438</v>
+      </c>
+      <c r="D175" t="s">
         <v>440</v>
       </c>
-      <c r="C175" t="s">
+      <c r="E175" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>197</v>
+      </c>
+      <c r="B176" t="s">
         <v>439</v>
       </c>
-      <c r="D175" t="s">
-        <v>441</v>
-      </c>
-      <c r="E175" t="s">
+      <c r="C176" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B176" t="s">
-        <v>440</v>
-      </c>
-      <c r="C176" t="s">
+      <c r="D176" s="4" t="s">
         <v>443</v>
-      </c>
-      <c r="D176" s="4" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -4590,24 +4731,27 @@
         <v>134</v>
       </c>
       <c r="B177" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C177" t="s">
+        <v>444</v>
+      </c>
+      <c r="D177" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="D177" s="4" t="s">
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>198</v>
+      </c>
+      <c r="B178" t="s">
+        <v>439</v>
+      </c>
+      <c r="C178" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B178" t="s">
-        <v>440</v>
-      </c>
-      <c r="C178" t="s">
+      <c r="D178" s="4" t="s">
         <v>447</v>
-      </c>
-      <c r="D178" s="4" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
@@ -4615,16 +4759,16 @@
         <v>127</v>
       </c>
       <c r="B179" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C179" t="s">
+        <v>448</v>
+      </c>
+      <c r="D179" t="s">
         <v>449</v>
       </c>
-      <c r="D179" t="s">
-        <v>450</v>
-      </c>
       <c r="E179" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
@@ -4632,16 +4776,16 @@
         <v>94</v>
       </c>
       <c r="B180" t="s">
+        <v>451</v>
+      </c>
+      <c r="C180" t="s">
+        <v>450</v>
+      </c>
+      <c r="D180" t="s">
         <v>452</v>
       </c>
-      <c r="C180" t="s">
-        <v>451</v>
-      </c>
-      <c r="D180" t="s">
+      <c r="E180" t="s">
         <v>453</v>
-      </c>
-      <c r="E180" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
@@ -4649,13 +4793,13 @@
         <v>22</v>
       </c>
       <c r="B181" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C181" t="s">
+        <v>454</v>
+      </c>
+      <c r="D181" s="4" t="s">
         <v>455</v>
-      </c>
-      <c r="D181" s="4" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
@@ -4663,35 +4807,41 @@
         <v>84</v>
       </c>
       <c r="B182" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C182" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>187</v>
+      </c>
+      <c r="B183" t="s">
+        <v>451</v>
+      </c>
+      <c r="C183" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B183" t="s">
-        <v>452</v>
-      </c>
-      <c r="C183" t="s">
+      <c r="D183" t="s">
         <v>458</v>
       </c>
-      <c r="D183" t="s">
+      <c r="E183" t="s">
         <v>459</v>
       </c>
-      <c r="E183" t="s">
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>160</v>
+      </c>
+      <c r="B184" t="s">
+        <v>451</v>
+      </c>
+      <c r="C184" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B184" t="s">
-        <v>452</v>
-      </c>
-      <c r="C184" t="s">
+      <c r="D184" s="4" t="s">
         <v>461</v>
-      </c>
-      <c r="D184" s="4" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -4699,16 +4849,16 @@
         <v>108</v>
       </c>
       <c r="B185" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C185" t="s">
+        <v>462</v>
+      </c>
+      <c r="D185" t="s">
         <v>463</v>
       </c>
-      <c r="D185" t="s">
+      <c r="E185" t="s">
         <v>464</v>
-      </c>
-      <c r="E185" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="186" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -4716,13 +4866,13 @@
         <v>60</v>
       </c>
       <c r="B186" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C186" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="E186" t="s">
         <v>466</v>
-      </c>
-      <c r="E186" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -4730,13 +4880,13 @@
         <v>51</v>
       </c>
       <c r="B187" t="s">
+        <v>468</v>
+      </c>
+      <c r="C187" t="s">
+        <v>467</v>
+      </c>
+      <c r="E187" t="s">
         <v>469</v>
-      </c>
-      <c r="C187" t="s">
-        <v>468</v>
-      </c>
-      <c r="E187" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
@@ -4744,16 +4894,16 @@
         <v>145</v>
       </c>
       <c r="B188" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C188" t="s">
+        <v>470</v>
+      </c>
+      <c r="D188" t="s">
         <v>471</v>
       </c>
-      <c r="D188" t="s">
+      <c r="E188" t="s">
         <v>472</v>
-      </c>
-      <c r="E188" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="189" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -4761,13 +4911,13 @@
         <v>53</v>
       </c>
       <c r="B189" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C189" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="D189" s="4" t="s">
         <v>474</v>
-      </c>
-      <c r="D189" s="4" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -4775,16 +4925,16 @@
         <v>44</v>
       </c>
       <c r="B190" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C190" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D190" t="s">
+        <v>514</v>
+      </c>
+      <c r="E190" t="s">
         <v>515</v>
-      </c>
-      <c r="E190" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -4792,16 +4942,16 @@
         <v>35</v>
       </c>
       <c r="B191" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C191" t="s">
+        <v>478</v>
+      </c>
+      <c r="D191" t="s">
         <v>479</v>
       </c>
-      <c r="D191" t="s">
+      <c r="E191" t="s">
         <v>480</v>
-      </c>
-      <c r="E191" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -4809,16 +4959,16 @@
         <v>93</v>
       </c>
       <c r="B192" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C192" t="s">
+        <v>481</v>
+      </c>
+      <c r="D192" t="s">
         <v>482</v>
       </c>
-      <c r="D192" t="s">
+      <c r="E192" t="s">
         <v>483</v>
-      </c>
-      <c r="E192" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
@@ -4826,13 +4976,13 @@
         <v>88</v>
       </c>
       <c r="B193" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C193" t="s">
+        <v>484</v>
+      </c>
+      <c r="D193" s="4" t="s">
         <v>485</v>
-      </c>
-      <c r="D193" s="4" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -4840,16 +4990,16 @@
         <v>43</v>
       </c>
       <c r="B194" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C194" t="s">
+        <v>486</v>
+      </c>
+      <c r="D194" t="s">
         <v>487</v>
       </c>
-      <c r="D194" t="s">
+      <c r="E194" t="s">
         <v>488</v>
-      </c>
-      <c r="E194" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
@@ -4857,13 +5007,13 @@
         <v>17</v>
       </c>
       <c r="B195" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C195" t="s">
+        <v>489</v>
+      </c>
+      <c r="D195" s="4" t="s">
         <v>490</v>
-      </c>
-      <c r="D195" s="4" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
@@ -4871,30 +5021,33 @@
         <v>91</v>
       </c>
       <c r="B196" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C196" t="s">
+        <v>491</v>
+      </c>
+      <c r="D196" t="s">
         <v>492</v>
       </c>
-      <c r="D196" t="s">
+      <c r="E196" t="s">
         <v>493</v>
       </c>
-      <c r="E196" t="s">
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>171</v>
+      </c>
+      <c r="B197" t="s">
+        <v>468</v>
+      </c>
+      <c r="C197" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B197" t="s">
-        <v>469</v>
-      </c>
-      <c r="C197" t="s">
+      <c r="D197" t="s">
         <v>495</v>
       </c>
-      <c r="D197" t="s">
+      <c r="E197" t="s">
         <v>496</v>
-      </c>
-      <c r="E197" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
@@ -4902,10 +5055,10 @@
         <v>124</v>
       </c>
       <c r="B198" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C198" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D198" t="s">
         <v>67</v>
@@ -4922,13 +5075,16 @@
         <v>278</v>
       </c>
       <c r="C199" t="s">
+        <v>498</v>
+      </c>
+      <c r="D199" s="4" t="s">
         <v>499</v>
       </c>
-      <c r="D199" s="4" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>167</v>
+      </c>
       <c r="B200" t="s">
         <v>278</v>
       </c>
@@ -4936,7 +5092,7 @@
         <v>276</v>
       </c>
       <c r="D200" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E200" t="s">
         <v>277</v>
@@ -4950,13 +5106,13 @@
         <v>278</v>
       </c>
       <c r="C201" t="s">
+        <v>501</v>
+      </c>
+      <c r="D201" t="s">
         <v>502</v>
       </c>
-      <c r="D201" t="s">
+      <c r="E201" t="s">
         <v>503</v>
-      </c>
-      <c r="E201" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -4967,27 +5123,30 @@
         <v>278</v>
       </c>
       <c r="C202" t="s">
+        <v>504</v>
+      </c>
+      <c r="D202" t="s">
         <v>505</v>
       </c>
-      <c r="D202" t="s">
+      <c r="E202" t="s">
         <v>506</v>
       </c>
-      <c r="E202" t="s">
-        <v>507</v>
-      </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>177</v>
+      </c>
       <c r="B203" t="s">
         <v>136</v>
       </c>
       <c r="C203" t="s">
+        <v>507</v>
+      </c>
+      <c r="D203" t="s">
         <v>508</v>
       </c>
-      <c r="D203" t="s">
+      <c r="E203" t="s">
         <v>509</v>
-      </c>
-      <c r="E203" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -4998,10 +5157,10 @@
         <v>136</v>
       </c>
       <c r="C204" t="s">
+        <v>510</v>
+      </c>
+      <c r="D204" s="4" t="s">
         <v>511</v>
-      </c>
-      <c r="D204" s="4" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
@@ -5012,35 +5171,41 @@
         <v>136</v>
       </c>
       <c r="C205" t="s">
+        <v>512</v>
+      </c>
+      <c r="D205" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="D205" s="4" t="s">
-        <v>514</v>
-      </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>169</v>
+      </c>
       <c r="B206" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C206" t="s">
+        <v>516</v>
+      </c>
+      <c r="D206" t="s">
+        <v>476</v>
+      </c>
+      <c r="E206" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>190</v>
+      </c>
+      <c r="B207" t="s">
+        <v>518</v>
+      </c>
+      <c r="C207" t="s">
         <v>517</v>
       </c>
-      <c r="D206" t="s">
-        <v>477</v>
-      </c>
-      <c r="E206" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B207" t="s">
+      <c r="D207" s="4" t="s">
         <v>519</v>
-      </c>
-      <c r="C207" t="s">
-        <v>518</v>
-      </c>
-      <c r="D207" s="4" t="s">
-        <v>520</v>
       </c>
     </row>
   </sheetData>

</xml_diff>